<commit_message>
primeira parte do cadastro
</commit_message>
<xml_diff>
--- a/documents/GERADOR DE CÓDIGO DE BARRA.xlsm.xlsx
+++ b/documents/GERADOR DE CÓDIGO DE BARRA.xlsm.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\gerador-codigo\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\gerador-codigosku\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88FE3EBE-4A36-45C0-9498-FC51A8BB6158}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B7CF1F55-3D3B-448E-8E5A-B11D972F4670}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,6 @@
     <definedName name="TIPO">'Gerador de Código'!$C$7:$D$198</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -2344,7 +2343,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2431,24 +2430,28 @@
       <c r="B3" s="4"/>
       <c r="C3" s="7" t="str">
         <f>VLOOKUP(C5,MARCA,2)</f>
-        <v>Rovitex</v>
+        <v>Phox</v>
       </c>
       <c r="D3" s="8" t="str">
         <f>VLOOKUP(D5,TIPO,2)</f>
-        <v>Blusa Viscose</v>
-      </c>
-      <c r="E3" s="9">
-        <v>6131175</v>
+        <v>Polo</v>
+      </c>
+      <c r="E3" s="9" t="str">
+        <f>VLOOKUP(E5,MODELO,3)</f>
+        <v>Basic</v>
       </c>
       <c r="F3" s="8" t="str">
         <f>VLOOKUP(F5,COR,2)</f>
         <v>Preto</v>
       </c>
-      <c r="G3" s="8"/>
+      <c r="G3" s="9" t="str">
+        <f>VLOOKUP(G5,TAMANHO,2)</f>
+        <v>PP</v>
+      </c>
       <c r="H3" s="6"/>
       <c r="I3" s="44" t="str">
         <f>CONCATENATE(C3," ",D3," ",E3," ","",F3," ",G3)</f>
-        <v xml:space="preserve">Rovitex Blusa Viscose 6131175 Preto </v>
+        <v>Phox Polo Basic Preto PP</v>
       </c>
       <c r="J3" s="42"/>
       <c r="K3" s="42"/>
@@ -2512,22 +2515,24 @@
       <c r="A5" s="2"/>
       <c r="B5" s="4"/>
       <c r="C5" s="14">
-        <v>133</v>
+        <v>100</v>
       </c>
       <c r="D5" s="9">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="E5" s="9">
-        <v>233</v>
+        <v>100</v>
       </c>
       <c r="F5" s="9">
         <v>10</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="9">
+        <v>10</v>
+      </c>
       <c r="H5" s="6"/>
       <c r="I5" s="44" t="str">
         <f>CONCATENATE(C5,D5,E5,F5,G5)</f>
-        <v>1335323310</v>
+        <v>100101001010</v>
       </c>
       <c r="J5" s="42"/>
       <c r="K5" s="42"/>
@@ -32240,7 +32245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0"/>
+    <sheetView topLeftCell="B112" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>